<commit_message>
Converted Process from Sequence to Flowchart
</commit_message>
<xml_diff>
--- a/Data/Input/PaymentTransactionTypes.xlsx
+++ b/Data/Input/PaymentTransactionTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6B9620-2362-4FB9-A451-73A270C09462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C48104-E41F-4BBD-92A4-B6864C155786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-18120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment Types" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>eSW Return Refund</t>
   </si>
@@ -100,10 +100,46 @@
     <t>L~=IFERROR(VLOOKUP($C{0},Fraud!$C:$G,5,FALSE),"-")¶M~=IFERROR(VLOOKUP($C{0},donotprocess!$A:$B,{0},FALSE),"-")¶N~=IFERROR(VLOOKUP($C{0},'Email Refunds'!B:J,4,FALSE),"-")¶O~=IFERROR(VLOOKUP($C{0},'MR-FIN'!C:K,4,FALSE),"-")</t>
   </si>
   <si>
-    <t>K~=LOOKUP(9.9E+307,--LEFT(MID(I{0},MIN(FIND({1,2,3,4,5,6,7,8,9,0}, $I{0}&amp;"1023456789")),999),ROW(INDIRECT("1:999"))))¶L~=RIGHT(I{0},LEN(I{0})-FIND(" ",I{0},1))¶M~=IFERROR(VLOOKUP($C{0},donotprocess!$A:$B,{0},FALSE),"-")¶N~=IFERROR(VLOOKUP($C{0},Fraud!$C:$G,5,FALSE),"-")¶O~=IFERROR(VLOOKUP($C{0},MR-FINC:(E),3,FALSE),"-")</t>
-  </si>
-  <si>
-    <t>N~=IFERROR(VLOOKUP(C{0},Fraud!C:G,5,FALSE),"-")</t>
+    <t>Fraud Column</t>
+  </si>
+  <si>
+    <t>Bank Details Changed Column</t>
+  </si>
+  <si>
+    <t>M~=IFERROR(VLOOKUP(C{0},'Email Refunds'!E:H,4,FALSE),"-")¶N~=IFERROR(VLOOKUP(C{0},Fraud!C:G,5,FALSE),"-")</t>
+  </si>
+  <si>
+    <t>K~=LOOKUP(9.9E+307,--LEFT(MID(I{0},MIN(FIND({1,2,3,4,5,6,7,8,9,0}, $I{0}&amp;"1023456789")),999),ROW(INDIRECT("1:999"))))¶L~=RIGHT(I{0},LEN(I{0})-FIND(" ",I{0},1))¶M~=IFERROR(VLOOKUP($C{0},donotprocess!$A:$B,{0},FALSE),"-")¶N~=IFERROR(VLOOKUP($C{0},Fraud!$C:$G,5,FALSE),"-")¶O~=IFERROR(VLOOKUP(C{0},'Refunds - FIN'!C:E,3,0),"-")</t>
+  </si>
+  <si>
+    <t>Last Column</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>FRAUD Check</t>
+  </si>
+  <si>
+    <t>Do not process</t>
+  </si>
+  <si>
+    <t>refunded by Fraud team?</t>
+  </si>
+  <si>
+    <t>Manual refunded Yes/No</t>
+  </si>
+  <si>
+    <t>Fraud</t>
+  </si>
+  <si>
+    <t>Manual refund</t>
   </si>
 </sst>
 </file>
@@ -421,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,9 +469,12 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -448,8 +487,17 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,8 +510,17 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -476,8 +533,17 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -490,8 +556,17 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -504,8 +579,17 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -518,8 +602,17 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -531,6 +624,15 @@
       </c>
       <c r="D7" t="s">
         <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -543,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D0C3AA-5529-4D71-AAA7-A99999E9619A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved forcing page size issue
</commit_message>
<xml_diff>
--- a/Data/Input/PaymentTransactionTypes.xlsx
+++ b/Data/Input/PaymentTransactionTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E5A61C-8126-4F58-A566-65DE39212BA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3BC3DE-7404-4F42-8F92-15C92A9E3146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment Types" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -509,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2925C6-D968-4F4F-941B-B3341CC9D29B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v1.0.43 config changed form UAT to Prod
</commit_message>
<xml_diff>
--- a/Data/Input/PaymentTransactionTypes.xlsx
+++ b/Data/Input/PaymentTransactionTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\VB\ESWNikeDailyRefunds\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726DDD29-C87E-4A93-944D-F697E28FDE16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F342280-2844-4E7A-9587-721C7DB2F87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment Types" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>eSW Return Refund</t>
   </si>
@@ -185,10 +185,10 @@
     <t>Authorisation,Processing,Status,Column1,Column2,Manual refund,Fraud,Column3,Refund Date</t>
   </si>
   <si>
-    <t>hiren.patel@uipath.com</t>
-  </si>
-  <si>
-    <t>Hiren Patel</t>
+    <t>cpujol@eshopworld.com</t>
+  </si>
+  <si>
+    <t>Carles Pujol</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -760,10 +760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2925C6-D968-4F4F-941B-B3341CC9D29B}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,19 +781,54 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3C55B9EA-3DE7-46C2-96CF-FFF9645FCDF2}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{75D60CB4-F1FB-4716-B224-0E7A089AB8E8}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{C17DC050-DAEA-4B60-9E67-FA991BD7DE74}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{15077B50-E36C-44CA-9F39-4E2A0A2A991B}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{3870C29F-0BA4-4F57-92F6-AA67C7161BF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -802,7 +837,7 @@
   <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:B4"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>